<commit_message>
Tests for isChecked Finished
Tests done and isChecked works correctly
</commit_message>
<xml_diff>
--- a/src/test/java/chess/possible checking positions.xlsx
+++ b/src/test/java/chess/possible checking positions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="21">
   <si>
     <t>K</t>
   </si>
@@ -37,6 +37,51 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Queen checking black King</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>&lt;-FALSE</t>
+  </si>
+  <si>
+    <t>Queen checking White King</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>Kn</t>
+  </si>
+  <si>
+    <t>Knight checking King</t>
+  </si>
+  <si>
+    <t>Do for both colors</t>
+  </si>
+  <si>
+    <t>Bishop checking king</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>&lt;-false</t>
+  </si>
+  <si>
+    <t>Do for both Colors</t>
+  </si>
+  <si>
+    <t>Rook checking king</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -92,8 +137,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -103,11 +154,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX22"/>
+  <dimension ref="A1:AY102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1046,7 +1103,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:50">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>3</v>
@@ -1060,7 +1117,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:50">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>4</v>
@@ -1074,7 +1131,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:50">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>5</v>
@@ -1088,7 +1145,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:50">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>6</v>
@@ -1102,7 +1159,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:50">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>7</v>
@@ -1116,7 +1173,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:50">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1127,6 +1184,4180 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:50">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1">
+        <v>6</v>
+      </c>
+      <c r="J23" s="1">
+        <v>7</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>4</v>
+      </c>
+      <c r="R23" s="1">
+        <v>5</v>
+      </c>
+      <c r="S23" s="1">
+        <v>6</v>
+      </c>
+      <c r="T23" s="1">
+        <v>7</v>
+      </c>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1">
+        <v>0</v>
+      </c>
+      <c r="X23" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN23" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AT23" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU23" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV23" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW23" s="1">
+        <v>6</v>
+      </c>
+      <c r="AX23" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:50">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AF24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+      <c r="AP24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+    </row>
+    <row r="25" spans="1:50">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="V25" s="1">
+        <v>1</v>
+      </c>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AF25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AP25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+    </row>
+    <row r="26" spans="1:50">
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="L26" s="1">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="V26" s="1">
+        <v>2</v>
+      </c>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AF26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AP26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="1"/>
+    </row>
+    <row r="27" spans="1:50">
+      <c r="B27" s="1">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="L27" s="1">
+        <v>3</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="V27" s="1">
+        <v>3</v>
+      </c>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AF27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="1"/>
+      <c r="AP27" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+    </row>
+    <row r="28" spans="1:50">
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="L28" s="1">
+        <v>4</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="V28" s="1">
+        <v>4</v>
+      </c>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AF28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="1"/>
+      <c r="AP28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+    </row>
+    <row r="29" spans="1:50">
+      <c r="B29" s="1">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="L29" s="1">
+        <v>5</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="V29" s="1">
+        <v>5</v>
+      </c>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AF29" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="1"/>
+      <c r="AP29" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="1"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+    </row>
+    <row r="30" spans="1:50">
+      <c r="B30" s="1">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1">
+        <v>6</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="V30" s="1">
+        <v>6</v>
+      </c>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AF30" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+      <c r="AL30" s="1"/>
+      <c r="AM30" s="1"/>
+      <c r="AN30" s="1"/>
+      <c r="AP30" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ30" s="1"/>
+      <c r="AR30" s="1"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="1"/>
+      <c r="AV30" s="1"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+    </row>
+    <row r="31" spans="1:50">
+      <c r="B31" s="1">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="L31" s="1">
+        <v>7</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="V31" s="1">
+        <v>7</v>
+      </c>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AF31" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+      <c r="AL31" s="1"/>
+      <c r="AM31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN31" s="1"/>
+      <c r="AP31" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ31" s="1"/>
+      <c r="AR31" s="1"/>
+      <c r="AS31" s="1"/>
+      <c r="AT31" s="1"/>
+      <c r="AU31" s="1"/>
+      <c r="AV31" s="1"/>
+      <c r="AW31" s="1"/>
+      <c r="AX31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:50">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4</v>
+      </c>
+      <c r="H33" s="1">
+        <v>5</v>
+      </c>
+      <c r="I33" s="1">
+        <v>6</v>
+      </c>
+      <c r="J33" s="1">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2</v>
+      </c>
+      <c r="P33" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>4</v>
+      </c>
+      <c r="R33" s="1">
+        <v>5</v>
+      </c>
+      <c r="S33" s="1">
+        <v>6</v>
+      </c>
+      <c r="T33" s="1">
+        <v>7</v>
+      </c>
+      <c r="U33" t="s">
+        <v>9</v>
+      </c>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1">
+        <v>0</v>
+      </c>
+      <c r="X33" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC33" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ33" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK33" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL33" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM33" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN33" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:50">
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="V34" s="1">
+        <v>0</v>
+      </c>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+      <c r="AK34" s="1"/>
+      <c r="AL34" s="1"/>
+      <c r="AM34" s="1"/>
+      <c r="AN34" s="1"/>
+    </row>
+    <row r="35" spans="2:50">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="V35" s="1">
+        <v>1</v>
+      </c>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AF35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="1"/>
+      <c r="AM35" s="1"/>
+      <c r="AN35" s="1"/>
+    </row>
+    <row r="36" spans="2:50">
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="L36" s="1">
+        <v>2</v>
+      </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="V36" s="1">
+        <v>2</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AF36" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1"/>
+    </row>
+    <row r="37" spans="2:50">
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="L37" s="1">
+        <v>3</v>
+      </c>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="V37" s="1">
+        <v>3</v>
+      </c>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AF37" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+      <c r="AL37" s="1"/>
+      <c r="AM37" s="1"/>
+      <c r="AN37" s="1"/>
+    </row>
+    <row r="38" spans="2:50">
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="L38" s="1">
+        <v>4</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="V38" s="1">
+        <v>4</v>
+      </c>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AF38" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG38" s="1"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="1"/>
+      <c r="AM38" s="1"/>
+      <c r="AN38" s="1"/>
+    </row>
+    <row r="39" spans="2:50">
+      <c r="B39" s="1">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="L39" s="1">
+        <v>5</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="V39" s="1">
+        <v>5</v>
+      </c>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AF39" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG39" s="1"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="1"/>
+      <c r="AM39" s="1"/>
+      <c r="AN39" s="1"/>
+    </row>
+    <row r="40" spans="2:50">
+      <c r="B40" s="1">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="L40" s="1">
+        <v>6</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="V40" s="1">
+        <v>6</v>
+      </c>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+      <c r="Z40" s="1"/>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AF40" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG40" s="1"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="1"/>
+      <c r="AM40" s="1"/>
+      <c r="AN40" s="1"/>
+    </row>
+    <row r="41" spans="2:50">
+      <c r="B41" s="1">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="L41" s="1">
+        <v>7</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V41" s="1">
+        <v>7</v>
+      </c>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AF41" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="1"/>
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+      <c r="AL41" s="1"/>
+      <c r="AM41" s="1"/>
+      <c r="AN41" s="1"/>
+    </row>
+    <row r="42" spans="2:50">
+      <c r="K42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:50">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1">
+        <v>4</v>
+      </c>
+      <c r="H43" s="1">
+        <v>5</v>
+      </c>
+      <c r="I43" s="1">
+        <v>6</v>
+      </c>
+      <c r="J43" s="1">
+        <v>7</v>
+      </c>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <v>1</v>
+      </c>
+      <c r="O43" s="1">
+        <v>2</v>
+      </c>
+      <c r="P43" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>4</v>
+      </c>
+      <c r="R43" s="1">
+        <v>5</v>
+      </c>
+      <c r="S43" s="1">
+        <v>6</v>
+      </c>
+      <c r="T43" s="1">
+        <v>7</v>
+      </c>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1">
+        <v>0</v>
+      </c>
+      <c r="X43" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB43" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC43" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF43" s="1"/>
+      <c r="AG43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK43" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL43" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM43" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN43" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP43" s="1"/>
+      <c r="AQ43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AT43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU43" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV43" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW43" s="1">
+        <v>6</v>
+      </c>
+      <c r="AX43" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:50">
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="L44" s="1">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V44" s="1">
+        <v>0</v>
+      </c>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AF44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="1"/>
+      <c r="AH44" s="1"/>
+      <c r="AI44" s="1"/>
+      <c r="AJ44" s="1"/>
+      <c r="AK44" s="1"/>
+      <c r="AL44" s="1"/>
+      <c r="AM44" s="1"/>
+      <c r="AN44" s="1"/>
+      <c r="AP44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ44" s="1"/>
+      <c r="AR44" s="1"/>
+      <c r="AS44" s="1"/>
+      <c r="AT44" s="1"/>
+      <c r="AU44" s="1"/>
+      <c r="AV44" s="1"/>
+      <c r="AW44" s="1"/>
+      <c r="AX44" s="1"/>
+    </row>
+    <row r="45" spans="2:50">
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="L45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="V45" s="1">
+        <v>1</v>
+      </c>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AF45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="1"/>
+      <c r="AH45" s="1"/>
+      <c r="AI45" s="1"/>
+      <c r="AJ45" s="1"/>
+      <c r="AK45" s="1"/>
+      <c r="AL45" s="1"/>
+      <c r="AM45" s="1"/>
+      <c r="AN45" s="1"/>
+      <c r="AP45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ45" s="1"/>
+      <c r="AR45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS45" s="1"/>
+      <c r="AT45" s="1"/>
+      <c r="AU45" s="1"/>
+      <c r="AV45" s="1"/>
+      <c r="AW45" s="1"/>
+      <c r="AX45" s="1"/>
+    </row>
+    <row r="46" spans="2:50">
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="L46" s="1">
+        <v>2</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="V46" s="1">
+        <v>2</v>
+      </c>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1"/>
+      <c r="AA46" s="1"/>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AF46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG46" s="1"/>
+      <c r="AH46" s="1"/>
+      <c r="AI46" s="1"/>
+      <c r="AJ46" s="1"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="1"/>
+      <c r="AM46" s="1"/>
+      <c r="AN46" s="1"/>
+      <c r="AP46" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ46" s="1"/>
+      <c r="AR46" s="1"/>
+      <c r="AS46" s="1"/>
+      <c r="AT46" s="1"/>
+      <c r="AU46" s="1"/>
+      <c r="AV46" s="1"/>
+      <c r="AW46" s="1"/>
+      <c r="AX46" s="1"/>
+    </row>
+    <row r="47" spans="2:50">
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="L47" s="1">
+        <v>3</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="V47" s="1">
+        <v>3</v>
+      </c>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AF47" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
+      <c r="AK47" s="1"/>
+      <c r="AL47" s="1"/>
+      <c r="AM47" s="1"/>
+      <c r="AN47" s="1"/>
+      <c r="AP47" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ47" s="1"/>
+      <c r="AR47" s="1"/>
+      <c r="AS47" s="1"/>
+      <c r="AT47" s="1"/>
+      <c r="AU47" s="1"/>
+      <c r="AV47" s="1"/>
+      <c r="AW47" s="1"/>
+      <c r="AX47" s="1"/>
+    </row>
+    <row r="48" spans="2:50">
+      <c r="B48" s="1">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="L48" s="1">
+        <v>4</v>
+      </c>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="V48" s="1">
+        <v>4</v>
+      </c>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AF48" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG48" s="1"/>
+      <c r="AH48" s="1"/>
+      <c r="AI48" s="1"/>
+      <c r="AJ48" s="1"/>
+      <c r="AK48" s="1"/>
+      <c r="AL48" s="1"/>
+      <c r="AM48" s="1"/>
+      <c r="AN48" s="1"/>
+      <c r="AP48" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ48" s="1"/>
+      <c r="AR48" s="1"/>
+      <c r="AS48" s="1"/>
+      <c r="AT48" s="1"/>
+      <c r="AU48" s="1"/>
+      <c r="AV48" s="1"/>
+      <c r="AW48" s="1"/>
+      <c r="AX48" s="1"/>
+    </row>
+    <row r="49" spans="2:50">
+      <c r="B49" s="1">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="L49" s="1">
+        <v>5</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="V49" s="1">
+        <v>5</v>
+      </c>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AF49" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG49" s="1"/>
+      <c r="AH49" s="1"/>
+      <c r="AI49" s="1"/>
+      <c r="AJ49" s="1"/>
+      <c r="AK49" s="1"/>
+      <c r="AL49" s="1"/>
+      <c r="AM49" s="1"/>
+      <c r="AN49" s="1"/>
+      <c r="AP49" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ49" s="1"/>
+      <c r="AR49" s="1"/>
+      <c r="AS49" s="1"/>
+      <c r="AT49" s="1"/>
+      <c r="AU49" s="1"/>
+      <c r="AV49" s="1"/>
+      <c r="AW49" s="1"/>
+      <c r="AX49" s="1"/>
+    </row>
+    <row r="50" spans="2:50">
+      <c r="B50" s="1">
+        <v>6</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="L50" s="1">
+        <v>6</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+      <c r="V50" s="1">
+        <v>6</v>
+      </c>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1"/>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AF50" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG50" s="1"/>
+      <c r="AH50" s="1"/>
+      <c r="AI50" s="1"/>
+      <c r="AJ50" s="1"/>
+      <c r="AK50" s="1"/>
+      <c r="AL50" s="1"/>
+      <c r="AM50" s="1"/>
+      <c r="AN50" s="1"/>
+      <c r="AP50" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ50" s="1"/>
+      <c r="AR50" s="1"/>
+      <c r="AS50" s="1"/>
+      <c r="AT50" s="1"/>
+      <c r="AU50" s="1"/>
+      <c r="AV50" s="1"/>
+      <c r="AW50" s="1"/>
+      <c r="AX50" s="1"/>
+    </row>
+    <row r="51" spans="2:50">
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="L51" s="1">
+        <v>7</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+      <c r="V51" s="1">
+        <v>7</v>
+      </c>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AF51" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH51" s="1"/>
+      <c r="AI51" s="1"/>
+      <c r="AJ51" s="1"/>
+      <c r="AK51" s="1"/>
+      <c r="AL51" s="1"/>
+      <c r="AM51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN51" s="1"/>
+      <c r="AP51" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ51" s="1"/>
+      <c r="AR51" s="1"/>
+      <c r="AS51" s="1"/>
+      <c r="AT51" s="1"/>
+      <c r="AU51" s="1"/>
+      <c r="AV51" s="1"/>
+      <c r="AW51" s="1"/>
+      <c r="AX51" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="2:50">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3</v>
+      </c>
+      <c r="G53" s="1">
+        <v>4</v>
+      </c>
+      <c r="H53" s="1">
+        <v>5</v>
+      </c>
+      <c r="I53" s="1">
+        <v>6</v>
+      </c>
+      <c r="J53" s="1">
+        <v>7</v>
+      </c>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1">
+        <v>0</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1</v>
+      </c>
+      <c r="O53" s="1">
+        <v>2</v>
+      </c>
+      <c r="P53" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>4</v>
+      </c>
+      <c r="R53" s="1">
+        <v>5</v>
+      </c>
+      <c r="S53" s="1">
+        <v>6</v>
+      </c>
+      <c r="T53" s="1">
+        <v>7</v>
+      </c>
+      <c r="U53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="2:50">
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+    </row>
+    <row r="55" spans="2:50">
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="L55" s="1">
+        <v>1</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
+      <c r="T55" s="1"/>
+    </row>
+    <row r="56" spans="2:50">
+      <c r="B56" s="1">
+        <v>2</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="L56" s="1">
+        <v>2</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+    </row>
+    <row r="57" spans="2:50">
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="L57" s="1">
+        <v>3</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+    </row>
+    <row r="58" spans="2:50">
+      <c r="B58" s="1">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="L58" s="1">
+        <v>4</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
+      <c r="T58" s="1"/>
+    </row>
+    <row r="59" spans="2:50">
+      <c r="B59" s="1">
+        <v>5</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="L59" s="1">
+        <v>5</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
+      <c r="T59" s="1"/>
+    </row>
+    <row r="60" spans="2:50">
+      <c r="B60" s="1">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="L60" s="1">
+        <v>6</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+    </row>
+    <row r="61" spans="2:50">
+      <c r="B61" s="1">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L61" s="1">
+        <v>7</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
+      <c r="T61" s="1"/>
+    </row>
+    <row r="62" spans="2:50">
+      <c r="K62" t="s">
+        <v>13</v>
+      </c>
+      <c r="U62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="2:50">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2</v>
+      </c>
+      <c r="F63" s="1">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1">
+        <v>4</v>
+      </c>
+      <c r="H63" s="1">
+        <v>5</v>
+      </c>
+      <c r="I63" s="1">
+        <v>6</v>
+      </c>
+      <c r="J63" s="1">
+        <v>7</v>
+      </c>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1">
+        <v>0</v>
+      </c>
+      <c r="N63" s="1">
+        <v>1</v>
+      </c>
+      <c r="O63" s="1">
+        <v>2</v>
+      </c>
+      <c r="P63" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>4</v>
+      </c>
+      <c r="R63" s="1">
+        <v>5</v>
+      </c>
+      <c r="S63" s="1">
+        <v>6</v>
+      </c>
+      <c r="T63" s="1">
+        <v>7</v>
+      </c>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1">
+        <v>0</v>
+      </c>
+      <c r="X63" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y63" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z63" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA63" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB63" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC63" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD63" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF63" s="1"/>
+      <c r="AG63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH63" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI63" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ63" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK63" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL63" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM63" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN63" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP63" s="1"/>
+      <c r="AQ63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR63" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS63" s="1">
+        <v>2</v>
+      </c>
+      <c r="AT63" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU63" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV63" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW63" s="1">
+        <v>6</v>
+      </c>
+      <c r="AX63" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="2:50">
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="V64" s="1">
+        <v>0</v>
+      </c>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
+      <c r="AF64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="1"/>
+      <c r="AH64" s="1"/>
+      <c r="AI64" s="1"/>
+      <c r="AJ64" s="1"/>
+      <c r="AK64" s="1"/>
+      <c r="AL64" s="1"/>
+      <c r="AM64" s="1"/>
+      <c r="AN64" s="1"/>
+      <c r="AP64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ64" s="1"/>
+      <c r="AR64" s="1"/>
+      <c r="AS64" s="1"/>
+      <c r="AT64" s="1"/>
+      <c r="AU64" s="1"/>
+      <c r="AV64" s="1"/>
+      <c r="AW64" s="1"/>
+      <c r="AX64" s="1"/>
+    </row>
+    <row r="65" spans="2:50">
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="L65" s="1">
+        <v>1</v>
+      </c>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="V65" s="1">
+        <v>1</v>
+      </c>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
+      <c r="AF65" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="1"/>
+      <c r="AH65" s="1"/>
+      <c r="AI65" s="1"/>
+      <c r="AJ65" s="1"/>
+      <c r="AK65" s="1"/>
+      <c r="AL65" s="1"/>
+      <c r="AM65" s="1"/>
+      <c r="AN65" s="1"/>
+      <c r="AP65" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ65" s="1"/>
+      <c r="AR65" s="1"/>
+      <c r="AS65" s="1"/>
+      <c r="AT65" s="1"/>
+      <c r="AU65" s="1"/>
+      <c r="AV65" s="1"/>
+      <c r="AW65" s="1"/>
+      <c r="AX65" s="1"/>
+    </row>
+    <row r="66" spans="2:50">
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="L66" s="1">
+        <v>2</v>
+      </c>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="V66" s="1">
+        <v>2</v>
+      </c>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AF66" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="1"/>
+      <c r="AP66" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ66" s="1"/>
+      <c r="AR66" s="1"/>
+      <c r="AS66" s="1"/>
+      <c r="AT66" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU66" s="1"/>
+      <c r="AV66" s="1"/>
+      <c r="AW66" s="1"/>
+      <c r="AX66" s="1"/>
+    </row>
+    <row r="67" spans="2:50">
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="L67" s="1">
+        <v>3</v>
+      </c>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="V67" s="1">
+        <v>3</v>
+      </c>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AF67" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG67" s="1"/>
+      <c r="AH67" s="1"/>
+      <c r="AI67" s="1"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+      <c r="AL67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM67" s="1"/>
+      <c r="AN67" s="1"/>
+      <c r="AP67" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ67" s="1"/>
+      <c r="AR67" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS67" s="1"/>
+      <c r="AT67" s="1"/>
+      <c r="AU67" s="1"/>
+      <c r="AV67" s="1"/>
+      <c r="AW67" s="1"/>
+      <c r="AX67" s="1"/>
+    </row>
+    <row r="68" spans="2:50">
+      <c r="B68" s="1">
+        <v>4</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="L68" s="1">
+        <v>4</v>
+      </c>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="T68" s="1"/>
+      <c r="V68" s="1">
+        <v>4</v>
+      </c>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
+      <c r="Z68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AF68" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG68" s="1"/>
+      <c r="AH68" s="1"/>
+      <c r="AI68" s="1"/>
+      <c r="AJ68" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK68" s="1"/>
+      <c r="AL68" s="1"/>
+      <c r="AM68" s="1"/>
+      <c r="AN68" s="1"/>
+      <c r="AP68" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ68" s="1"/>
+      <c r="AR68" s="1"/>
+      <c r="AS68" s="1"/>
+      <c r="AT68" s="1"/>
+      <c r="AU68" s="1"/>
+      <c r="AV68" s="1"/>
+      <c r="AW68" s="1"/>
+      <c r="AX68" s="1"/>
+    </row>
+    <row r="69" spans="2:50">
+      <c r="B69" s="1">
+        <v>5</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="L69" s="1">
+        <v>5</v>
+      </c>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="V69" s="1">
+        <v>5</v>
+      </c>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AF69" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG69" s="1"/>
+      <c r="AH69" s="1"/>
+      <c r="AI69" s="1"/>
+      <c r="AJ69" s="1"/>
+      <c r="AK69" s="1"/>
+      <c r="AL69" s="1"/>
+      <c r="AM69" s="1"/>
+      <c r="AN69" s="1"/>
+      <c r="AP69" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ69" s="1"/>
+      <c r="AR69" s="1"/>
+      <c r="AS69" s="1"/>
+      <c r="AT69" s="1"/>
+      <c r="AU69" s="1"/>
+      <c r="AV69" s="1"/>
+      <c r="AW69" s="1"/>
+      <c r="AX69" s="1"/>
+    </row>
+    <row r="70" spans="2:50">
+      <c r="B70" s="1">
+        <v>6</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="L70" s="1">
+        <v>6</v>
+      </c>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="V70" s="1">
+        <v>6</v>
+      </c>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AF70" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="1"/>
+      <c r="AM70" s="1"/>
+      <c r="AN70" s="1"/>
+      <c r="AP70" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ70" s="1"/>
+      <c r="AR70" s="1"/>
+      <c r="AS70" s="1"/>
+      <c r="AT70" s="1"/>
+      <c r="AU70" s="1"/>
+      <c r="AV70" s="1"/>
+      <c r="AW70" s="1"/>
+      <c r="AX70" s="1"/>
+    </row>
+    <row r="71" spans="2:50">
+      <c r="B71" s="1">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="L71" s="1">
+        <v>7</v>
+      </c>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="V71" s="1">
+        <v>7</v>
+      </c>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AF71" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
+      <c r="AJ71" s="1"/>
+      <c r="AK71" s="1"/>
+      <c r="AL71" s="1"/>
+      <c r="AM71" s="1"/>
+      <c r="AN71" s="1"/>
+      <c r="AP71" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ71" s="1"/>
+      <c r="AR71" s="1"/>
+      <c r="AS71" s="1"/>
+      <c r="AT71" s="1"/>
+      <c r="AU71" s="1"/>
+      <c r="AV71" s="1"/>
+      <c r="AW71" s="1"/>
+      <c r="AX71" s="1"/>
+    </row>
+    <row r="73" spans="2:50">
+      <c r="B73" s="1"/>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2</v>
+      </c>
+      <c r="F73" s="1">
+        <v>3</v>
+      </c>
+      <c r="G73" s="1">
+        <v>4</v>
+      </c>
+      <c r="H73" s="1">
+        <v>5</v>
+      </c>
+      <c r="I73" s="1">
+        <v>6</v>
+      </c>
+      <c r="J73" s="1">
+        <v>7</v>
+      </c>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1">
+        <v>0</v>
+      </c>
+      <c r="N73" s="1">
+        <v>1</v>
+      </c>
+      <c r="O73" s="1">
+        <v>2</v>
+      </c>
+      <c r="P73" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>4</v>
+      </c>
+      <c r="R73" s="1">
+        <v>5</v>
+      </c>
+      <c r="S73" s="1">
+        <v>6</v>
+      </c>
+      <c r="T73" s="1">
+        <v>7</v>
+      </c>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1">
+        <v>0</v>
+      </c>
+      <c r="X73" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA73" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB73" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC73" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="2:50">
+      <c r="B74" s="1">
+        <v>0</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="L74" s="1">
+        <v>0</v>
+      </c>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="V74" s="1">
+        <v>0</v>
+      </c>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+    </row>
+    <row r="75" spans="2:50">
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="L75" s="1">
+        <v>1</v>
+      </c>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="V75" s="1">
+        <v>1</v>
+      </c>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+      <c r="Z75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA75" s="1"/>
+      <c r="AB75" s="1"/>
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+    </row>
+    <row r="76" spans="2:50">
+      <c r="B76" s="1">
+        <v>2</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="L76" s="1">
+        <v>2</v>
+      </c>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R76" s="1"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="1"/>
+      <c r="V76" s="1">
+        <v>2</v>
+      </c>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
+      <c r="Z76" s="1"/>
+      <c r="AA76" s="1"/>
+      <c r="AB76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+    </row>
+    <row r="77" spans="2:50">
+      <c r="B77" s="1">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="L77" s="1">
+        <v>3</v>
+      </c>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="1"/>
+      <c r="V77" s="1">
+        <v>3</v>
+      </c>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
+      <c r="Z77" s="1"/>
+      <c r="AA77" s="1"/>
+      <c r="AB77" s="1"/>
+      <c r="AC77" s="1"/>
+      <c r="AD77" s="1"/>
+    </row>
+    <row r="78" spans="2:50">
+      <c r="B78" s="1">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="L78" s="1">
+        <v>4</v>
+      </c>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="V78" s="1">
+        <v>4</v>
+      </c>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
+      <c r="Z78" s="1"/>
+      <c r="AA78" s="1"/>
+      <c r="AB78" s="1"/>
+      <c r="AC78" s="1"/>
+      <c r="AD78" s="1"/>
+    </row>
+    <row r="79" spans="2:50">
+      <c r="B79" s="1">
+        <v>5</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="L79" s="1">
+        <v>5</v>
+      </c>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="V79" s="1">
+        <v>5</v>
+      </c>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
+      <c r="Z79" s="1"/>
+      <c r="AA79" s="1"/>
+      <c r="AB79" s="1"/>
+      <c r="AC79" s="1"/>
+      <c r="AD79" s="1"/>
+    </row>
+    <row r="80" spans="2:50">
+      <c r="B80" s="1">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="L80" s="1">
+        <v>6</v>
+      </c>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="V80" s="1">
+        <v>6</v>
+      </c>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+      <c r="AA80" s="1"/>
+      <c r="AB80" s="1"/>
+      <c r="AC80" s="1"/>
+      <c r="AD80" s="1"/>
+    </row>
+    <row r="81" spans="2:51">
+      <c r="B81" s="1">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="L81" s="1">
+        <v>7</v>
+      </c>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="1"/>
+      <c r="T81" s="1"/>
+      <c r="V81" s="1">
+        <v>7</v>
+      </c>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+      <c r="Y81" s="1"/>
+      <c r="Z81" s="1"/>
+      <c r="AA81" s="1"/>
+      <c r="AB81" s="1"/>
+      <c r="AC81" s="1"/>
+      <c r="AD81" s="1"/>
+    </row>
+    <row r="83" spans="2:51">
+      <c r="K83" t="s">
+        <v>15</v>
+      </c>
+      <c r="U83" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="2:51">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2</v>
+      </c>
+      <c r="F84" s="1">
+        <v>3</v>
+      </c>
+      <c r="G84" s="1">
+        <v>4</v>
+      </c>
+      <c r="H84" s="1">
+        <v>5</v>
+      </c>
+      <c r="I84" s="1">
+        <v>6</v>
+      </c>
+      <c r="J84" s="1">
+        <v>7</v>
+      </c>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1">
+        <v>0</v>
+      </c>
+      <c r="N84" s="1">
+        <v>1</v>
+      </c>
+      <c r="O84" s="1">
+        <v>2</v>
+      </c>
+      <c r="P84" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>4</v>
+      </c>
+      <c r="R84" s="1">
+        <v>5</v>
+      </c>
+      <c r="S84" s="1">
+        <v>6</v>
+      </c>
+      <c r="T84" s="1">
+        <v>7</v>
+      </c>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1">
+        <v>0</v>
+      </c>
+      <c r="X84" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y84" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z84" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA84" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB84" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC84" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD84" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF84" s="1"/>
+      <c r="AG84" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI84" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ84" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK84" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL84" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM84" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN84" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP84" s="1"/>
+      <c r="AQ84" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR84" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS84" s="1">
+        <v>2</v>
+      </c>
+      <c r="AT84" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU84" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV84" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW84" s="1">
+        <v>6</v>
+      </c>
+      <c r="AX84" s="1">
+        <v>7</v>
+      </c>
+      <c r="AY84" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="2:51">
+      <c r="B85" s="1">
+        <v>0</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="L85" s="1">
+        <v>0</v>
+      </c>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="1"/>
+      <c r="T85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V85" s="1">
+        <v>0</v>
+      </c>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
+      <c r="Z85" s="1"/>
+      <c r="AA85" s="1"/>
+      <c r="AB85" s="1"/>
+      <c r="AC85" s="1"/>
+      <c r="AD85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF85" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH85" s="1"/>
+      <c r="AI85" s="1"/>
+      <c r="AJ85" s="1"/>
+      <c r="AK85" s="1"/>
+      <c r="AL85" s="1"/>
+      <c r="AM85" s="1"/>
+      <c r="AN85" s="1"/>
+      <c r="AP85" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR85" s="1"/>
+      <c r="AS85" s="1"/>
+      <c r="AT85" s="1"/>
+      <c r="AU85" s="1"/>
+      <c r="AV85" s="1"/>
+      <c r="AW85" s="1"/>
+      <c r="AX85" s="1"/>
+    </row>
+    <row r="86" spans="2:51">
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="L86" s="1">
+        <v>1</v>
+      </c>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="V86" s="1">
+        <v>1</v>
+      </c>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
+      <c r="Z86" s="1"/>
+      <c r="AA86" s="1"/>
+      <c r="AB86" s="1"/>
+      <c r="AC86" s="1"/>
+      <c r="AD86" s="1"/>
+      <c r="AF86" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG86" s="1"/>
+      <c r="AH86" s="1"/>
+      <c r="AI86" s="1"/>
+      <c r="AJ86" s="1"/>
+      <c r="AK86" s="1"/>
+      <c r="AL86" s="1"/>
+      <c r="AM86" s="1"/>
+      <c r="AN86" s="1"/>
+      <c r="AP86" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ86" s="1"/>
+      <c r="AR86" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS86" s="1"/>
+      <c r="AT86" s="1"/>
+      <c r="AU86" s="1"/>
+      <c r="AV86" s="1"/>
+      <c r="AW86" s="1"/>
+      <c r="AX86" s="1"/>
+    </row>
+    <row r="87" spans="2:51">
+      <c r="B87" s="1">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="L87" s="1">
+        <v>2</v>
+      </c>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="V87" s="1">
+        <v>2</v>
+      </c>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
+      <c r="Z87" s="1"/>
+      <c r="AA87" s="1"/>
+      <c r="AB87" s="1"/>
+      <c r="AC87" s="1"/>
+      <c r="AD87" s="1"/>
+      <c r="AF87" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG87" s="1"/>
+      <c r="AH87" s="1"/>
+      <c r="AI87" s="1"/>
+      <c r="AJ87" s="1"/>
+      <c r="AK87" s="1"/>
+      <c r="AL87" s="1"/>
+      <c r="AM87" s="1"/>
+      <c r="AN87" s="1"/>
+      <c r="AP87" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ87" s="1"/>
+      <c r="AR87" s="1"/>
+      <c r="AS87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT87" s="1"/>
+      <c r="AU87" s="1"/>
+      <c r="AV87" s="1"/>
+      <c r="AW87" s="1"/>
+      <c r="AX87" s="1"/>
+    </row>
+    <row r="88" spans="2:51">
+      <c r="B88" s="1">
+        <v>3</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="L88" s="1">
+        <v>3</v>
+      </c>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="V88" s="1">
+        <v>3</v>
+      </c>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
+      <c r="Z88" s="1"/>
+      <c r="AA88" s="1"/>
+      <c r="AB88" s="1"/>
+      <c r="AC88" s="1"/>
+      <c r="AD88" s="1"/>
+      <c r="AF88" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG88" s="1"/>
+      <c r="AH88" s="1"/>
+      <c r="AI88" s="1"/>
+      <c r="AJ88" s="1"/>
+      <c r="AK88" s="1"/>
+      <c r="AL88" s="1"/>
+      <c r="AM88" s="1"/>
+      <c r="AN88" s="1"/>
+      <c r="AP88" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ88" s="1"/>
+      <c r="AR88" s="1"/>
+      <c r="AS88" s="1"/>
+      <c r="AT88" s="1"/>
+      <c r="AU88" s="1"/>
+      <c r="AV88" s="1"/>
+      <c r="AW88" s="1"/>
+      <c r="AX88" s="1"/>
+    </row>
+    <row r="89" spans="2:51">
+      <c r="B89" s="1">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="L89" s="1">
+        <v>4</v>
+      </c>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="V89" s="1">
+        <v>4</v>
+      </c>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+      <c r="Y89" s="1"/>
+      <c r="Z89" s="1"/>
+      <c r="AA89" s="1"/>
+      <c r="AB89" s="1"/>
+      <c r="AC89" s="1"/>
+      <c r="AD89" s="1"/>
+      <c r="AF89" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG89" s="1"/>
+      <c r="AH89" s="1"/>
+      <c r="AI89" s="1"/>
+      <c r="AJ89" s="1"/>
+      <c r="AK89" s="1"/>
+      <c r="AL89" s="1"/>
+      <c r="AM89" s="1"/>
+      <c r="AN89" s="1"/>
+      <c r="AP89" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ89" s="1"/>
+      <c r="AR89" s="1"/>
+      <c r="AS89" s="1"/>
+      <c r="AT89" s="1"/>
+      <c r="AU89" s="1"/>
+      <c r="AV89" s="1"/>
+      <c r="AW89" s="1"/>
+      <c r="AX89" s="1"/>
+    </row>
+    <row r="90" spans="2:51">
+      <c r="B90" s="1">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="L90" s="1">
+        <v>5</v>
+      </c>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="V90" s="1">
+        <v>5</v>
+      </c>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
+      <c r="Z90" s="1"/>
+      <c r="AA90" s="1"/>
+      <c r="AB90" s="1"/>
+      <c r="AC90" s="1"/>
+      <c r="AD90" s="1"/>
+      <c r="AF90" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG90" s="1"/>
+      <c r="AH90" s="1"/>
+      <c r="AI90" s="1"/>
+      <c r="AJ90" s="1"/>
+      <c r="AK90" s="1"/>
+      <c r="AL90" s="1"/>
+      <c r="AM90" s="1"/>
+      <c r="AN90" s="1"/>
+      <c r="AP90" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ90" s="1"/>
+      <c r="AR90" s="1"/>
+      <c r="AS90" s="1"/>
+      <c r="AT90" s="1"/>
+      <c r="AU90" s="1"/>
+      <c r="AV90" s="1"/>
+      <c r="AW90" s="1"/>
+      <c r="AX90" s="1"/>
+    </row>
+    <row r="91" spans="2:51">
+      <c r="B91" s="1">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="L91" s="1">
+        <v>6</v>
+      </c>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="V91" s="1">
+        <v>6</v>
+      </c>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+      <c r="AA91" s="1"/>
+      <c r="AB91" s="1"/>
+      <c r="AC91" s="1"/>
+      <c r="AD91" s="1"/>
+      <c r="AF91" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG91" s="1"/>
+      <c r="AH91" s="1"/>
+      <c r="AI91" s="1"/>
+      <c r="AJ91" s="1"/>
+      <c r="AK91" s="1"/>
+      <c r="AL91" s="1"/>
+      <c r="AM91" s="1"/>
+      <c r="AN91" s="1"/>
+      <c r="AP91" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ91" s="1"/>
+      <c r="AR91" s="1"/>
+      <c r="AS91" s="1"/>
+      <c r="AT91" s="1"/>
+      <c r="AU91" s="1"/>
+      <c r="AV91" s="1"/>
+      <c r="AW91" s="1"/>
+      <c r="AX91" s="1"/>
+    </row>
+    <row r="92" spans="2:51">
+      <c r="B92" s="1">
+        <v>7</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L92" s="1">
+        <v>7</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="V92" s="1">
+        <v>7</v>
+      </c>
+      <c r="W92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
+      <c r="Z92" s="1"/>
+      <c r="AA92" s="1"/>
+      <c r="AB92" s="1"/>
+      <c r="AC92" s="1"/>
+      <c r="AD92" s="1"/>
+      <c r="AF92" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG92" s="1"/>
+      <c r="AH92" s="1"/>
+      <c r="AI92" s="1"/>
+      <c r="AJ92" s="1"/>
+      <c r="AK92" s="1"/>
+      <c r="AL92" s="1"/>
+      <c r="AM92" s="1"/>
+      <c r="AN92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP92" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ92" s="1"/>
+      <c r="AR92" s="1"/>
+      <c r="AS92" s="1"/>
+      <c r="AT92" s="1"/>
+      <c r="AU92" s="1"/>
+      <c r="AV92" s="1"/>
+      <c r="AW92" s="1"/>
+      <c r="AX92" s="1"/>
+    </row>
+    <row r="93" spans="2:51">
+      <c r="K93" t="s">
+        <v>19</v>
+      </c>
+      <c r="U93" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="2:51">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1</v>
+      </c>
+      <c r="E94" s="1">
+        <v>2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3</v>
+      </c>
+      <c r="G94" s="1">
+        <v>4</v>
+      </c>
+      <c r="H94" s="1">
+        <v>5</v>
+      </c>
+      <c r="I94" s="1">
+        <v>6</v>
+      </c>
+      <c r="J94" s="1">
+        <v>7</v>
+      </c>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1">
+        <v>0</v>
+      </c>
+      <c r="N94" s="1">
+        <v>1</v>
+      </c>
+      <c r="O94" s="1">
+        <v>2</v>
+      </c>
+      <c r="P94" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>4</v>
+      </c>
+      <c r="R94" s="1">
+        <v>5</v>
+      </c>
+      <c r="S94" s="1">
+        <v>6</v>
+      </c>
+      <c r="T94" s="1">
+        <v>7</v>
+      </c>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1">
+        <v>0</v>
+      </c>
+      <c r="X94" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y94" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z94" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA94" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB94" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC94" s="1">
+        <v>6</v>
+      </c>
+      <c r="AD94" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF94" s="1"/>
+      <c r="AG94" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH94" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI94" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ94" s="1">
+        <v>3</v>
+      </c>
+      <c r="AK94" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL94" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM94" s="1">
+        <v>6</v>
+      </c>
+      <c r="AN94" s="1">
+        <v>7</v>
+      </c>
+      <c r="AP94" s="1"/>
+      <c r="AQ94" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR94" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS94" s="1">
+        <v>2</v>
+      </c>
+      <c r="AT94" s="1">
+        <v>3</v>
+      </c>
+      <c r="AU94" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV94" s="1">
+        <v>5</v>
+      </c>
+      <c r="AW94" s="1">
+        <v>6</v>
+      </c>
+      <c r="AX94" s="1">
+        <v>7</v>
+      </c>
+      <c r="AY94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="2:51">
+      <c r="B95" s="1">
+        <v>0</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="L95" s="1">
+        <v>0</v>
+      </c>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T95" s="1"/>
+      <c r="V95" s="1">
+        <v>0</v>
+      </c>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+      <c r="AA95" s="1"/>
+      <c r="AB95" s="1"/>
+      <c r="AC95" s="1"/>
+      <c r="AD95" s="1"/>
+      <c r="AF95" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG95" s="1"/>
+      <c r="AH95" s="1"/>
+      <c r="AI95" s="1"/>
+      <c r="AJ95" s="1"/>
+      <c r="AK95" s="1"/>
+      <c r="AL95" s="1"/>
+      <c r="AM95" s="1"/>
+      <c r="AN95" s="1"/>
+      <c r="AP95" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ95" s="1"/>
+      <c r="AR95" s="1"/>
+      <c r="AS95" s="1"/>
+      <c r="AT95" s="1"/>
+      <c r="AU95" s="1"/>
+      <c r="AV95" s="1"/>
+      <c r="AW95" s="1"/>
+      <c r="AX95" s="1"/>
+    </row>
+    <row r="96" spans="2:51">
+      <c r="B96" s="1">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="L96" s="1">
+        <v>1</v>
+      </c>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="V96" s="1">
+        <v>1</v>
+      </c>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+      <c r="Z96" s="1"/>
+      <c r="AA96" s="1"/>
+      <c r="AB96" s="1"/>
+      <c r="AC96" s="1"/>
+      <c r="AD96" s="1"/>
+      <c r="AF96" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG96" s="1"/>
+      <c r="AH96" s="1"/>
+      <c r="AI96" s="1"/>
+      <c r="AJ96" s="1"/>
+      <c r="AK96" s="1"/>
+      <c r="AL96" s="1"/>
+      <c r="AM96" s="1"/>
+      <c r="AN96" s="1"/>
+      <c r="AP96" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ96" s="1"/>
+      <c r="AR96" s="1"/>
+      <c r="AS96" s="1"/>
+      <c r="AT96" s="1"/>
+      <c r="AU96" s="1"/>
+      <c r="AV96" s="1"/>
+      <c r="AW96" s="1"/>
+      <c r="AX96" s="1"/>
+    </row>
+    <row r="97" spans="2:50">
+      <c r="B97" s="1">
+        <v>2</v>
+      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="L97" s="1">
+        <v>2</v>
+      </c>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="V97" s="1">
+        <v>2</v>
+      </c>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+      <c r="Z97" s="1"/>
+      <c r="AA97" s="1"/>
+      <c r="AB97" s="1"/>
+      <c r="AC97" s="1"/>
+      <c r="AD97" s="1"/>
+      <c r="AF97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG97" s="1"/>
+      <c r="AH97" s="1"/>
+      <c r="AI97" s="1"/>
+      <c r="AJ97" s="1"/>
+      <c r="AK97" s="1"/>
+      <c r="AL97" s="1"/>
+      <c r="AM97" s="1"/>
+      <c r="AN97" s="1"/>
+      <c r="AP97" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ97" s="1"/>
+      <c r="AR97" s="1"/>
+      <c r="AS97" s="1"/>
+      <c r="AT97" s="1"/>
+      <c r="AU97" s="1"/>
+      <c r="AV97" s="1"/>
+      <c r="AW97" s="1"/>
+      <c r="AX97" s="1"/>
+    </row>
+    <row r="98" spans="2:50">
+      <c r="B98" s="1">
+        <v>3</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="L98" s="1">
+        <v>3</v>
+      </c>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="V98" s="1">
+        <v>3</v>
+      </c>
+      <c r="W98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
+      <c r="Z98" s="1"/>
+      <c r="AA98" s="1"/>
+      <c r="AB98" s="1"/>
+      <c r="AC98" s="1"/>
+      <c r="AD98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF98" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH98" s="1"/>
+      <c r="AI98" s="1"/>
+      <c r="AJ98" s="1"/>
+      <c r="AK98" s="1"/>
+      <c r="AL98" s="1"/>
+      <c r="AM98" s="1"/>
+      <c r="AN98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP98" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR98" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS98" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT98" s="1"/>
+      <c r="AU98" s="1"/>
+      <c r="AV98" s="1"/>
+      <c r="AW98" s="1"/>
+      <c r="AX98" s="1"/>
+    </row>
+    <row r="99" spans="2:50">
+      <c r="B99" s="1">
+        <v>4</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="L99" s="1">
+        <v>4</v>
+      </c>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
+      <c r="V99" s="1">
+        <v>4</v>
+      </c>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
+      <c r="Z99" s="1"/>
+      <c r="AA99" s="1"/>
+      <c r="AB99" s="1"/>
+      <c r="AC99" s="1"/>
+      <c r="AD99" s="1"/>
+      <c r="AF99" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG99" s="1"/>
+      <c r="AH99" s="1"/>
+      <c r="AI99" s="1"/>
+      <c r="AJ99" s="1"/>
+      <c r="AK99" s="1"/>
+      <c r="AL99" s="1"/>
+      <c r="AM99" s="1"/>
+      <c r="AN99" s="1"/>
+      <c r="AP99" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ99" s="1"/>
+      <c r="AR99" s="1"/>
+      <c r="AS99" s="1"/>
+      <c r="AT99" s="1"/>
+      <c r="AU99" s="1"/>
+      <c r="AV99" s="1"/>
+      <c r="AW99" s="1"/>
+      <c r="AX99" s="1"/>
+    </row>
+    <row r="100" spans="2:50">
+      <c r="B100" s="1">
+        <v>5</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="L100" s="1">
+        <v>5</v>
+      </c>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="V100" s="1">
+        <v>5</v>
+      </c>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+      <c r="Z100" s="1"/>
+      <c r="AA100" s="1"/>
+      <c r="AB100" s="1"/>
+      <c r="AC100" s="1"/>
+      <c r="AD100" s="1"/>
+      <c r="AF100" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG100" s="1"/>
+      <c r="AH100" s="1"/>
+      <c r="AI100" s="1"/>
+      <c r="AJ100" s="1"/>
+      <c r="AK100" s="1"/>
+      <c r="AL100" s="1"/>
+      <c r="AM100" s="1"/>
+      <c r="AN100" s="1"/>
+      <c r="AP100" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ100" s="1"/>
+      <c r="AR100" s="1"/>
+      <c r="AS100" s="1"/>
+      <c r="AT100" s="1"/>
+      <c r="AU100" s="1"/>
+      <c r="AV100" s="1"/>
+      <c r="AW100" s="1"/>
+      <c r="AX100" s="1"/>
+    </row>
+    <row r="101" spans="2:50">
+      <c r="B101" s="1">
+        <v>6</v>
+      </c>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="L101" s="1">
+        <v>6</v>
+      </c>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="V101" s="1">
+        <v>6</v>
+      </c>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
+      <c r="AA101" s="1"/>
+      <c r="AB101" s="1"/>
+      <c r="AC101" s="1"/>
+      <c r="AD101" s="1"/>
+      <c r="AF101" s="1">
+        <v>6</v>
+      </c>
+      <c r="AG101" s="1"/>
+      <c r="AH101" s="1"/>
+      <c r="AI101" s="1"/>
+      <c r="AJ101" s="1"/>
+      <c r="AK101" s="1"/>
+      <c r="AL101" s="1"/>
+      <c r="AM101" s="1"/>
+      <c r="AN101" s="1"/>
+      <c r="AP101" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ101" s="1"/>
+      <c r="AR101" s="1"/>
+      <c r="AS101" s="1"/>
+      <c r="AT101" s="1"/>
+      <c r="AU101" s="1"/>
+      <c r="AV101" s="1"/>
+      <c r="AW101" s="1"/>
+      <c r="AX101" s="1"/>
+    </row>
+    <row r="102" spans="2:50">
+      <c r="B102" s="1">
+        <v>7</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="L102" s="1">
+        <v>7</v>
+      </c>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+      <c r="S102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T102" s="1"/>
+      <c r="V102" s="1">
+        <v>7</v>
+      </c>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
+      <c r="Z102" s="1"/>
+      <c r="AA102" s="1"/>
+      <c r="AB102" s="1"/>
+      <c r="AC102" s="1"/>
+      <c r="AD102" s="1"/>
+      <c r="AF102" s="1">
+        <v>7</v>
+      </c>
+      <c r="AG102" s="1"/>
+      <c r="AH102" s="1"/>
+      <c r="AI102" s="1"/>
+      <c r="AJ102" s="1"/>
+      <c r="AK102" s="1"/>
+      <c r="AL102" s="1"/>
+      <c r="AM102" s="1"/>
+      <c r="AN102" s="1"/>
+      <c r="AP102" s="1">
+        <v>7</v>
+      </c>
+      <c r="AQ102" s="1"/>
+      <c r="AR102" s="1"/>
+      <c r="AS102" s="1"/>
+      <c r="AT102" s="1"/>
+      <c r="AU102" s="1"/>
+      <c r="AV102" s="1"/>
+      <c r="AW102" s="1"/>
+      <c r="AX102" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>